<commit_message>
Added code for data provider
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/uiAutomation/data/TestData.xlsx
+++ b/src/main/java/com/test/automation/uiAutomation/data/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
@@ -385,7 +385,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adding code for Test Base
</commit_message>
<xml_diff>
--- a/src/main/java/com/test/automation/uiAutomation/data/TestData.xlsx
+++ b/src/main/java/com/test/automation/uiAutomation/data/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>userName</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -385,7 +388,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -434,7 +437,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -445,7 +448,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -456,7 +459,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -467,7 +470,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>